<commit_message>
here modified myexcel file
</commit_message>
<xml_diff>
--- a/sampleexcel.xlsx
+++ b/sampleexcel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\git\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333DCD1A-4894-4892-877B-A697A2451FF0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,46 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>CONTACT</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>ROHIT KAWADE</t>
+  </si>
+  <si>
+    <t>rohitkawade021@gmail.com</t>
+  </si>
+  <si>
+    <t>ROLL</t>
+  </si>
+  <si>
+    <t>//EDITED THID FILE ALSO</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,13 +86,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +373,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>9822907360</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{019FFAF4-F7C4-49C3-B9FB-FE30BD475D24}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>